<commit_message>
feat: realize the pos machine using tasking diagram
</commit_message>
<xml_diff>
--- a/timelog.xlsx
+++ b/timelog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JYang53\Desktop\TW homework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JYang53\Desktop\TW homework\Day1\POS-Machine-V1-2020-11-5-3-48-45-545\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E338346-2C2D-4510-9C24-6A73F3C6E40D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EC35E64B-BF44-4734-BB00-0AE7505FDD0D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="504" windowWidth="28800" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>W</t>
   </si>
@@ -131,6 +131,10 @@
       </rPr>
       <t>Action: maybe this task is not appropraite. Maybe I need more practice to improve my coding basic</t>
     </r>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>processInput(new)</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -854,11 +858,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
@@ -1052,8 +1056,12 @@
         <f>WEEKNUM(Template!$E5)</f>
         <v>0</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="17">
+        <v>20</v>
+      </c>
       <c r="D5" s="4" t="str">
         <f>IF(ISBLANK(Template!$F5),"",((Template!$F5-Template!$E5)))</f>
         <v/>

</xml_diff>